<commit_message>
dev : dynamics identification
</commit_message>
<xml_diff>
--- a/src/saber_control/src/saber_fourier_series.xlsx
+++ b/src/saber_control/src/saber_fourier_series.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="12080"/>
+    <workbookView windowWidth="28800" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -967,342 +967,342 @@
   <dimension ref="A1:A66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A1" sqref="A1:A66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="29.8727272727273" customWidth="1"/>
+    <col min="1" max="1" width="29.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" ht="15" spans="1:1">
       <c r="A1" s="1">
-        <v>-0.0649715650631648</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
+        <v>0.00333938462730028</v>
+      </c>
+    </row>
+    <row r="2" ht="15" spans="1:1">
       <c r="A2" s="1">
-        <v>0.107772071352337</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+        <v>0.00333384923609884</v>
+      </c>
+    </row>
+    <row r="3" ht="15" spans="1:1">
       <c r="A3" s="1">
-        <v>-0.969128584533121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
+        <v>-0.0483427458717823</v>
+      </c>
+    </row>
+    <row r="4" ht="15" spans="1:1">
       <c r="A4" s="1">
-        <v>0.087106940209473</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
+        <v>-0.260456087909828</v>
+      </c>
+    </row>
+    <row r="5" ht="15" spans="1:1">
       <c r="A5" s="1">
-        <v>0.839221138037786</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
+        <v>0.300859661366</v>
+      </c>
+    </row>
+    <row r="6" ht="15" spans="1:1">
       <c r="A6" s="1">
-        <v>0.147464147440916</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
+        <v>0.0489348920394959</v>
+      </c>
+    </row>
+    <row r="7" ht="15" spans="1:1">
       <c r="A7" s="1">
-        <v>-0.292464125417334</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
+        <v>0.029475024446471</v>
+      </c>
+    </row>
+    <row r="8" ht="15" spans="1:1">
       <c r="A8" s="1">
-        <v>0.0662814000438366</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
+        <v>-0.153092694500051</v>
+      </c>
+    </row>
+    <row r="9" ht="15" spans="1:1">
       <c r="A9" s="1">
-        <v>-0.354926620627601</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
+        <v>-0.634042080077492</v>
+      </c>
+    </row>
+    <row r="10" ht="15" spans="1:1">
       <c r="A10" s="1">
-        <v>0.33166527715477</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
+        <v>0.576915794297815</v>
+      </c>
+    </row>
+    <row r="11" ht="15" spans="1:1">
       <c r="A11" s="1">
-        <v>0.00295163989385672</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
+        <v>-0.0982900850264507</v>
+      </c>
+    </row>
+    <row r="12" ht="15" spans="1:1">
       <c r="A12" s="1">
-        <v>0.0929832985681864</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
+        <v>0.0168622783694167</v>
+      </c>
+    </row>
+    <row r="13" ht="15" spans="1:1">
       <c r="A13" s="1">
-        <v>0.175648364428025</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
+        <v>-0.294824039207678</v>
+      </c>
+    </row>
+    <row r="14" ht="15" spans="1:1">
       <c r="A14" s="1">
-        <v>0.00112325079399384</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
+        <v>-0.256542767097894</v>
+      </c>
+    </row>
+    <row r="15" ht="15" spans="1:1">
       <c r="A15" s="1">
-        <v>0.217211029786139</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
+        <v>0.294017335906422</v>
+      </c>
+    </row>
+    <row r="16" ht="15" spans="1:1">
       <c r="A16" s="1">
-        <v>-0.486965943576798</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
+        <v>0.240015488168106</v>
+      </c>
+    </row>
+    <row r="17" ht="15" spans="1:1">
       <c r="A17" s="1">
-        <v>-0.0175791772358718</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
+        <v>0.121912319763234</v>
+      </c>
+    </row>
+    <row r="18" ht="15" spans="1:1">
       <c r="A18" s="1">
-        <v>0.153186850161474</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
+        <v>-0.163786511095751</v>
+      </c>
+    </row>
+    <row r="19" ht="15" spans="1:1">
       <c r="A19" s="1">
-        <v>0.167628498379024</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
+        <v>0.0298695983684544</v>
+      </c>
+    </row>
+    <row r="20" ht="15" spans="1:1">
       <c r="A20" s="1">
-        <v>-0.504617414199301</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
+        <v>0.113952178280737</v>
+      </c>
+    </row>
+    <row r="21" ht="15" spans="1:1">
       <c r="A21" s="1">
-        <v>0.245357927712691</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
+        <v>-0.0677709101145603</v>
+      </c>
+    </row>
+    <row r="22" ht="15" spans="1:1">
       <c r="A22" s="1">
-        <v>-1.45045085196156</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
+        <v>-1.36269842684397</v>
+      </c>
+    </row>
+    <row r="23" ht="15" spans="1:1">
       <c r="A23" s="1">
-        <v>-0.0821677513625397</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
+        <v>0.00720203280867843</v>
+      </c>
+    </row>
+    <row r="24" ht="15" spans="1:1">
       <c r="A24" s="1">
-        <v>-0.116771757580566</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
+        <v>0.106061171029263</v>
+      </c>
+    </row>
+    <row r="25" ht="15" spans="1:1">
       <c r="A25" s="1">
-        <v>0.0232123701922822</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
+        <v>0.572283564124571</v>
+      </c>
+    </row>
+    <row r="26" ht="15" spans="1:1">
       <c r="A26" s="1">
-        <v>-0.38455349271258</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
+        <v>-0.0228043935037851</v>
+      </c>
+    </row>
+    <row r="27" ht="15" spans="1:1">
       <c r="A27" s="1">
-        <v>0.560280631466054</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
+        <v>-0.662615245731844</v>
+      </c>
+    </row>
+    <row r="28" ht="15" spans="1:1">
       <c r="A28" s="1">
-        <v>0.0264495284052431</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
+        <v>-0.138223596050814</v>
+      </c>
+    </row>
+    <row r="29" ht="15" spans="1:1">
       <c r="A29" s="1">
-        <v>-0.157112880513458</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
+        <v>0.170728474434344</v>
+      </c>
+    </row>
+    <row r="30" ht="15" spans="1:1">
       <c r="A30" s="1">
-        <v>-0.173434846763802</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
+        <v>-0.0205234267280683</v>
+      </c>
+    </row>
+    <row r="31" ht="15" spans="1:1">
       <c r="A31" s="1">
-        <v>0.345218580278064</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
+        <v>0.0592439574360344</v>
+      </c>
+    </row>
+    <row r="32" ht="15" spans="1:1">
       <c r="A32" s="1">
-        <v>-0.114558709637501</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
+        <v>-0.0757318073806069</v>
+      </c>
+    </row>
+    <row r="33" ht="15" spans="1:1">
       <c r="A33" s="1">
-        <v>-0.14809566174419</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
+        <v>-0.192509243285872</v>
+      </c>
+    </row>
+    <row r="34" ht="15" spans="1:1">
       <c r="A34" s="1">
-        <v>0.0568241934998166</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
+        <v>-0.00856878590228507</v>
+      </c>
+    </row>
+    <row r="35" ht="15" spans="1:1">
       <c r="A35" s="1">
-        <v>-0.1646497459798</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
+        <v>-0.00335629421967389</v>
+      </c>
+    </row>
+    <row r="36" ht="15" spans="1:1">
       <c r="A36" s="1">
-        <v>0.0586459762390444</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
+        <v>0.0049403279019122</v>
+      </c>
+    </row>
+    <row r="37" ht="15" spans="1:1">
       <c r="A37" s="1">
-        <v>-0.325824738799826</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
+        <v>0.00477108920676527</v>
+      </c>
+    </row>
+    <row r="38" ht="15" spans="1:1">
       <c r="A38" s="1">
-        <v>0.375004315043687</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
+        <v>0.00249855438070927</v>
+      </c>
+    </row>
+    <row r="39" ht="15" spans="1:1">
       <c r="A39" s="1">
-        <v>-0.0925318497423989</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
+        <v>0.0141936891896592</v>
+      </c>
+    </row>
+    <row r="40" ht="15" spans="1:1">
       <c r="A40" s="1">
-        <v>-0.0293618709324146</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
+        <v>0.0606428150431505</v>
+      </c>
+    </row>
+    <row r="41" ht="15" spans="1:1">
       <c r="A41" s="1">
-        <v>0.426626362197345</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
+        <v>-0.189228986429901</v>
+      </c>
+    </row>
+    <row r="42" ht="15" spans="1:1">
       <c r="A42" s="1">
-        <v>0.0782647755908338</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
+        <v>-0.535933094740337</v>
+      </c>
+    </row>
+    <row r="43" ht="15" spans="1:1">
       <c r="A43" s="1">
-        <v>-0.288336519468179</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
+        <v>0.51501576930382</v>
+      </c>
+    </row>
+    <row r="44" ht="15" spans="1:1">
       <c r="A44" s="1">
-        <v>-1.58068019191218</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
+        <v>-1.72841212132103</v>
+      </c>
+    </row>
+    <row r="45" ht="15" spans="1:1">
       <c r="A45" s="1">
-        <v>-0.0656028622462553</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
+        <v>0.0309928744032121</v>
+      </c>
+    </row>
+    <row r="46" ht="15" spans="1:1">
       <c r="A46" s="1">
-        <v>0.346262586831496</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
+        <v>0.0231946587797607</v>
+      </c>
+    </row>
+    <row r="47" ht="15" spans="1:1">
       <c r="A47" s="1">
-        <v>-0.204013365992958</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
+        <v>0.532433526864129</v>
+      </c>
+    </row>
+    <row r="48" ht="15" spans="1:1">
       <c r="A48" s="1">
-        <v>0.391946001460968</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
+        <v>0.0993388500174188</v>
+      </c>
+    </row>
+    <row r="49" ht="15" spans="1:1">
       <c r="A49" s="1">
-        <v>-0.468592360048508</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
+        <v>-0.685814933112209</v>
+      </c>
+    </row>
+    <row r="50" ht="15" spans="1:1">
       <c r="A50" s="1">
-        <v>-0.110457974859375</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
+        <v>0.0472789852553486</v>
+      </c>
+    </row>
+    <row r="51" ht="15" spans="1:1">
       <c r="A51" s="1">
-        <v>0.380841009659672</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
+        <v>-0.158064460956765</v>
+      </c>
+    </row>
+    <row r="52" ht="15" spans="1:1">
       <c r="A52" s="1">
-        <v>0.315784404379584</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
+        <v>0.33475202890947</v>
+      </c>
+    </row>
+    <row r="53" ht="15" spans="1:1">
       <c r="A53" s="1">
-        <v>-0.00802632404042166</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
+        <v>-0.175539468648756</v>
+      </c>
+    </row>
+    <row r="54" ht="15" spans="1:1">
       <c r="A54" s="1">
-        <v>-0.313294392284099</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
+        <v>-0.00672581926646901</v>
+      </c>
+    </row>
+    <row r="55" ht="15" spans="1:1">
       <c r="A55" s="1">
-        <v>0.383749747101452</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
+        <v>0.110485505289996</v>
+      </c>
+    </row>
+    <row r="56" ht="15" spans="1:1">
       <c r="A56" s="1">
-        <v>0.273051735097086</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
+        <v>0.0509580994017887</v>
+      </c>
+    </row>
+    <row r="57" ht="15" spans="1:1">
       <c r="A57" s="1">
-        <v>0.58218592648069</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
+        <v>-0.191448426500055</v>
+      </c>
+    </row>
+    <row r="58" ht="15" spans="1:1">
       <c r="A58" s="1">
-        <v>-0.0671417335508825</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1">
+        <v>-0.244909277698867</v>
+      </c>
+    </row>
+    <row r="59" ht="15" spans="1:1">
       <c r="A59" s="1">
-        <v>-0.0701646878044179</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1">
+        <v>0.215353666982259</v>
+      </c>
+    </row>
+    <row r="60" ht="15" spans="1:1">
       <c r="A60" s="1">
-        <v>-0.717931240222481</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1">
+        <v>0.170094141643033</v>
+      </c>
+    </row>
+    <row r="61" ht="15" spans="1:1">
       <c r="A61" s="1">
-        <v>-0.0721732906935152</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1">
+        <v>0.458711201908083</v>
+      </c>
+    </row>
+    <row r="62" ht="15" spans="1:1">
       <c r="A62" s="1">
-        <v>0.705623761268585</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1">
+        <v>-0.738979774779363</v>
+      </c>
+    </row>
+    <row r="63" ht="15" spans="1:1">
       <c r="A63" s="1">
-        <v>-0.685352009612478</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
+        <v>-0.54694756176714</v>
+      </c>
+    </row>
+    <row r="64" ht="15" spans="1:1">
       <c r="A64" s="1">
-        <v>-0.0941582948991534</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1">
+        <v>0.378313949612719</v>
+      </c>
+    </row>
+    <row r="65" ht="15" spans="1:1">
       <c r="A65" s="1">
-        <v>0.218722995316269</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
+        <v>0.229283012855533</v>
+      </c>
+    </row>
+    <row r="66" ht="15" spans="1:1">
       <c r="A66" s="1">
-        <v>0.23043390213139</v>
+        <v>0.152315742160172</v>
       </c>
     </row>
   </sheetData>
@@ -1321,7 +1321,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1338,7 +1338,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>